<commit_message>
Guardando cambios antes de hacer pull
</commit_message>
<xml_diff>
--- a/datos/codigos.xlsx
+++ b/datos/codigos.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Adrian\Documents\2024_Python\SEPT_PYTHON\LESSON11\Buscador_de_ID\datos\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{161E8F0E-0286-4DDE-98E3-391BCAF1A5C8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A82E96DC-8950-4CFC-BA03-B52458F7E6B3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{0509E686-CFE0-492B-83C0-EF772D7D3B85}"/>
   </bookViews>
@@ -25,12 +25,9 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2" uniqueCount="2">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1" uniqueCount="1">
   <si>
     <t>Expediente</t>
-  </si>
-  <si>
-    <t>PF_PITEIB-10/2024</t>
   </si>
 </sst>
 </file>
@@ -428,11 +425,6 @@
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A2" t="s">
-        <v>1</v>
-      </c>
-    </row>
     <row r="42" spans="4:4" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="43" spans="4:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="D43" s="2"/>

</xml_diff>